<commit_message>
ENH: Added pytest cases.
</commit_message>
<xml_diff>
--- a/testdata/sales.xlsx
+++ b/testdata/sales.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="sales" sheetId="1" state="visible" r:id="rId2"/>
@@ -132,6 +132,7 @@
       <color rgb="FF000000"/>
       <name val="Microsoft YaHei"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -234,16 +235,16 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -820,12 +821,12 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -919,17 +920,17 @@
   </sheetPr>
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>21</v>
       </c>
@@ -937,7 +938,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
         <v>43101</v>
       </c>
@@ -945,9 +946,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
-        <f aca="false">A2+1</f>
         <v>43102</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -955,9 +955,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="n">
-        <f aca="false">A3+1</f>
         <v>43103</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -965,9 +964,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
-        <f aca="false">A4+1</f>
         <v>43104</v>
       </c>
       <c r="B5" s="0" t="n">
@@ -975,9 +973,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
-        <f aca="false">A5+1</f>
         <v>43105</v>
       </c>
       <c r="B6" s="0" t="n">
@@ -985,9 +982,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="n">
-        <f aca="false">A6+1</f>
         <v>43106</v>
       </c>
       <c r="B7" s="0" t="n">
@@ -995,9 +991,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
-        <f aca="false">A7+1</f>
         <v>43107</v>
       </c>
       <c r="B8" s="0" t="n">
@@ -1005,9 +1000,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
-        <f aca="false">A8+1</f>
         <v>43108</v>
       </c>
       <c r="B9" s="0" t="n">
@@ -1015,9 +1009,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="n">
-        <f aca="false">A9+1</f>
         <v>43109</v>
       </c>
       <c r="B10" s="0" t="n">
@@ -1025,9 +1018,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="n">
-        <f aca="false">A10+1</f>
         <v>43110</v>
       </c>
       <c r="B11" s="0" t="n">
@@ -1035,9 +1027,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="n">
-        <f aca="false">A11+1</f>
         <v>43111</v>
       </c>
       <c r="B12" s="0" t="n">
@@ -1045,9 +1036,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="n">
-        <f aca="false">A12+1</f>
         <v>43112</v>
       </c>
       <c r="B13" s="0" t="n">
@@ -1055,9 +1045,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="n">
-        <f aca="false">A13+1</f>
         <v>43113</v>
       </c>
       <c r="B14" s="0" t="n">
@@ -1065,9 +1054,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="n">
-        <f aca="false">A14+1</f>
         <v>43114</v>
       </c>
       <c r="B15" s="0" t="n">
@@ -1075,9 +1063,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="n">
-        <f aca="false">A15+1</f>
         <v>43115</v>
       </c>
       <c r="B16" s="0" t="n">
@@ -1085,9 +1072,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="n">
-        <f aca="false">A16+1</f>
         <v>43116</v>
       </c>
       <c r="B17" s="0" t="n">
@@ -1095,9 +1081,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="n">
-        <f aca="false">A17+1</f>
         <v>43117</v>
       </c>
       <c r="B18" s="0" t="n">
@@ -1105,9 +1090,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="n">
-        <f aca="false">A18+1</f>
         <v>43118</v>
       </c>
       <c r="B19" s="0" t="n">
@@ -1115,9 +1099,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="n">
-        <f aca="false">A19+1</f>
         <v>43119</v>
       </c>
       <c r="B20" s="0" t="n">
@@ -1125,9 +1108,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="n">
-        <f aca="false">A20+1</f>
         <v>43120</v>
       </c>
       <c r="B21" s="0" t="n">
@@ -1135,9 +1117,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="n">
-        <f aca="false">A21+1</f>
         <v>43121</v>
       </c>
       <c r="B22" s="0" t="n">
@@ -1145,9 +1126,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="n">
-        <f aca="false">A22+1</f>
         <v>43122</v>
       </c>
       <c r="B23" s="0" t="n">
@@ -1155,9 +1135,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="n">
-        <f aca="false">A23+1</f>
         <v>43123</v>
       </c>
       <c r="B24" s="0" t="n">
@@ -1165,9 +1144,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="n">
-        <f aca="false">A24+1</f>
         <v>43124</v>
       </c>
       <c r="B25" s="0" t="n">
@@ -1175,9 +1153,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="n">
-        <f aca="false">A25+1</f>
         <v>43125</v>
       </c>
       <c r="B26" s="0" t="n">
@@ -1185,9 +1162,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="n">
-        <f aca="false">A26+1</f>
         <v>43126</v>
       </c>
       <c r="B27" s="0" t="n">
@@ -1195,9 +1171,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="n">
-        <f aca="false">A27+1</f>
         <v>43127</v>
       </c>
       <c r="B28" s="0" t="n">
@@ -1205,9 +1180,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="n">
-        <f aca="false">A28+1</f>
         <v>43128</v>
       </c>
       <c r="B29" s="0" t="n">
@@ -1215,9 +1189,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="n">
-        <f aca="false">A29+1</f>
         <v>43129</v>
       </c>
       <c r="B30" s="0" t="n">
@@ -1225,9 +1198,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="n">
-        <f aca="false">A30+1</f>
         <v>43130</v>
       </c>
       <c r="B31" s="0" t="n">
@@ -1235,9 +1207,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="n">
-        <f aca="false">A31+1</f>
         <v>43131</v>
       </c>
       <c r="B32" s="0" t="n">
@@ -1245,9 +1216,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="n">
-        <f aca="false">A32+1</f>
         <v>43132</v>
       </c>
       <c r="B33" s="0" t="n">
@@ -1255,9 +1225,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="n">
-        <f aca="false">A33+1</f>
         <v>43133</v>
       </c>
       <c r="B34" s="0" t="n">
@@ -1289,7 +1258,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>